<commit_message>
added initial report and rmd
</commit_message>
<xml_diff>
--- a/nfhs3-analysis/Household.xlsx
+++ b/nfhs3-analysis/Household.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" tabRatio="550" firstSheet="35" activeTab="37"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" tabRatio="550" firstSheet="30" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="HV201DWS" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="135">
   <si>
     <t>Urban</t>
   </si>
@@ -441,9 +441,6 @@
     <t>SH56C/Window screens</t>
   </si>
   <si>
-    <t>SH56A/Glass windows</t>
-  </si>
-  <si>
     <t>SH56D/Window with curtain or shutters</t>
   </si>
   <si>
@@ -463,6 +460,12 @@
   </si>
   <si>
     <t>Don't know</t>
+  </si>
+  <si>
+    <t>HV243B/Watch</t>
+  </si>
+  <si>
+    <t>SH56B/Glass windows</t>
   </si>
 </sst>
 </file>
@@ -3440,7 +3443,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="A1:I16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3452,7 +3455,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="16" t="s">
@@ -11438,6 +11441,9 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A25:B25"/>
@@ -11446,24 +11452,13 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:G21"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C20:G20"/>
@@ -11472,6 +11467,14 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17020,8 +17023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17033,7 +17036,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="16" t="s">
@@ -17835,7 +17838,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="16" t="s">
@@ -18236,7 +18239,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="16" t="s">
@@ -18295,7 +18298,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="13">
@@ -18322,7 +18325,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="13">
@@ -18507,7 +18510,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="16" t="s">
@@ -18895,7 +18898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -18908,7 +18911,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="16" t="s">
@@ -18967,7 +18970,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="13">
@@ -19197,7 +19200,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="13">

</xml_diff>